<commit_message>
Mudança nos usuarios da planilha
</commit_message>
<xml_diff>
--- a/Cópia de clientes.xlsx
+++ b/Cópia de clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismar\Desktop\automaçao-py\Automa-o-em-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24F52156-561B-4001-90BC-96BEDBFF9CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A455BA5-07C5-4539-95E4-42E59A05794B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nome</t>
   </si>
@@ -45,16 +45,13 @@
     <t>vencimento</t>
   </si>
   <si>
-    <t>Luciano</t>
-  </si>
-  <si>
     <t>Ismar pai</t>
   </si>
   <si>
     <t>Rejania</t>
   </si>
   <si>
-    <t>Augusto</t>
+    <t>Marília Lucí</t>
   </si>
 </sst>
 </file>
@@ -415,7 +412,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -436,18 +433,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
-        <v>558396234059</v>
+        <v>558388008228</v>
       </c>
       <c r="C2" s="2">
-        <v>45991</v>
+        <v>45839</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>558399965073</v>
@@ -458,25 +455,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>558396234059</v>
+        <v>5583987592215</v>
       </c>
       <c r="C4" s="2">
         <v>45993</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>558396117591</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45994</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>

</xml_diff>